<commit_message>
final commit to finish first usable version
</commit_message>
<xml_diff>
--- a/devdoc/Zeiterfassung.xlsx
+++ b/devdoc/Zeiterfassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\java\studium\sensemaker\devdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAA016F1-A9D1-49BC-A02D-8B74A1E21F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1EA8E0-1CCB-4CF2-95E8-6B21BF246997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2178" yWindow="1374" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2148" yWindow="1068" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitliste" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -320,15 +320,6 @@
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -343,6 +334,15 @@
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +464,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Experimentieren</c:v>
+                  <c:v>DAL Impl.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -493,7 +493,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,7 +522,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fxml Experimente</c:v>
+                  <c:v>DAL Planung</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -551,7 +551,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -580,7 +580,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Recherche</c:v>
+                  <c:v>DAL Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -609,7 +609,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -638,7 +638,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Setup</c:v>
+                  <c:v>Experimentieren</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -667,7 +667,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -696,7 +696,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Touch Experimente</c:v>
+                  <c:v>Frontend</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -725,7 +725,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,28 +957,33 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daglemino" refreshedDate="44000.407352546295" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daglemino" refreshedDate="44000.464083680556" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2020-04-12T00:00:00" maxDate="2020-05-20T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2020-04-12T00:00:00" maxDate="2020-06-18T00:00:00"/>
     </cacheField>
     <cacheField name="Uhrzeit" numFmtId="0">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T09:00:00" maxDate="1899-12-30T16:00:00"/>
     </cacheField>
     <cacheField name="Endzeit" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T10:00:00" maxDate="1899-12-30T17:30:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T10:00:00" maxDate="1899-12-30T21:00:00"/>
     </cacheField>
     <cacheField name="Tätigkeit" numFmtId="0">
-      <sharedItems containsBlank="1" count="12">
+      <sharedItems containsBlank="1" count="17">
         <s v="Recherche"/>
         <s v="Setup"/>
         <s v="Experimentieren"/>
         <s v="Touch Experimente"/>
         <s v="fxml Experimente"/>
         <s v="Business-Layer"/>
+        <s v="DAL Planung"/>
+        <s v="DAL Impl."/>
+        <s v="DAL Testing"/>
+        <s v="MVVM impl."/>
+        <s v="Frontend"/>
         <m/>
         <s v="Deployment" u="1"/>
         <s v="Meeting" u="1"/>
@@ -988,7 +993,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Dauer (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="4.5"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="44.5"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1059,982 +1064,982 @@
   </r>
   <r>
     <d v="2020-05-17T00:00:00"/>
-    <m/>
-    <m/>
+    <d v="1899-12-30T15:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
     <x v="6"/>
-    <m/>
+    <n v="1"/>
   </r>
   <r>
     <d v="2020-05-19T00:00:00"/>
     <d v="1899-12-30T13:00:00"/>
     <d v="1899-12-30T15:00:00"/>
-    <x v="6"/>
+    <x v="7"/>
     <n v="2"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <x v="6"/>
+    <d v="2020-06-14T00:00:00"/>
+    <d v="1899-12-30T14:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <x v="7"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <d v="2020-06-15T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <x v="8"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <d v="2020-06-16T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <x v="9"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <d v="2020-06-17T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <x v="10"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <n v="44.5"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
     <m/>
   </r>
 </pivotCacheRecords>
@@ -2042,25 +2047,30 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Zeitliste Pivot" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" compact="0" compactData="0">
-  <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A1:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField name="Datum" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0" includeNewItemsInFilter="1"/>
     <pivotField compact="0" outline="0" showAll="0" includeNewItemsInFilter="1"/>
     <pivotField name="Tätigkeit" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="13">
+      <items count="18">
         <item x="5"/>
-        <item m="1" x="7"/>
-        <item m="1" x="11"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item m="1" x="12"/>
+        <item m="1" x="16"/>
         <item x="2"/>
+        <item x="10"/>
         <item x="4"/>
-        <item m="1" x="10"/>
-        <item m="1" x="8"/>
+        <item m="1" x="15"/>
+        <item m="1" x="13"/>
+        <item x="9"/>
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="9"/>
+        <item m="1" x="14"/>
         <item x="3"/>
-        <item x="6"/>
+        <item x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2069,15 +2079,21 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="13">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
     </i>
     <i>
-      <x v="4"/>
+      <x v="6"/>
     </i>
     <i>
       <x v="7"/>
@@ -2086,10 +2102,19 @@
       <x v="8"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="11"/>
     </i>
     <i>
-      <x v="11"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
     </i>
     <i t="grand">
       <x/>
@@ -2424,13 +2449,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -2440,18 +2465,18 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -2704,7 +2729,7 @@
       <c r="A17" s="14">
         <v>43997</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="21">
         <v>0.45833333333333331</v>
       </c>
       <c r="C17" s="16">
@@ -2724,7 +2749,7 @@
       <c r="A18" s="14">
         <v>43998</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="21">
         <v>0.54166666666666663</v>
       </c>
       <c r="C18" s="16">
@@ -2744,7 +2769,7 @@
       <c r="A19" s="14">
         <v>43999</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="21">
         <v>0.45833333333333331</v>
       </c>
       <c r="C19" s="16">
@@ -3744,7 +3769,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -3762,10 +3787,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="18">
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -3773,59 +3798,99 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B6" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A4" s="22" t="s">
+    <row r="7" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B8" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A5" s="22" t="s">
+    <row r="9" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A9" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B10" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A6" s="22" t="s">
+    <row r="11" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B11" s="20">
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A7" s="22" t="s">
+    <row r="12" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B12" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A8" s="22" t="s">
+    <row r="13" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
+      <c r="B13" s="20">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="13">
-        <v>16.5</v>
+      <c r="B14" s="13">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>